<commit_message>
Calculation of ES working
</commit_message>
<xml_diff>
--- a/PMConverter/administration/2_Project data input sheet_extended_checked.xlsx
+++ b/PMConverter/administration/2_Project data input sheet_extended_checked.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36165" yWindow="-5595" windowWidth="29340" windowHeight="16440" tabRatio="628" activeTab="6"/>
+    <workbookView xWindow="-36165" yWindow="-5595" windowWidth="29340" windowHeight="16440" tabRatio="628" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline Schedule" sheetId="1" r:id="rId1"/>
@@ -1627,7 +1627,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1756,6 +1756,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="120">
@@ -31506,8 +31512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -31531,7 +31537,8 @@
     <col min="19" max="20" width="9" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -33039,8 +33046,8 @@
         <v>0.97</v>
       </c>
       <c r="V19" s="3"/>
-      <c r="W19" s="5">
-        <v>542212.4375</v>
+      <c r="W19" s="52">
+        <v>528148.41970322584</v>
       </c>
       <c r="X19" s="5">
         <v>542212.4375</v>
@@ -33126,8 +33133,8 @@
       <c r="V20" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="W20" s="9">
-        <v>143670.9062</v>
+      <c r="W20" s="51">
+        <v>129606.87270322582</v>
       </c>
       <c r="X20" s="9">
         <v>143670.9062</v>
@@ -37221,7 +37228,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -37230,7 +37237,7 @@
   <dimension ref="A1:AJ63"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -37254,7 +37261,8 @@
     <col min="19" max="20" width="9" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.375" customWidth="1"/>
   </cols>
@@ -39238,8 +39246,8 @@
         <v>0.99</v>
       </c>
       <c r="V24" s="3"/>
-      <c r="W24" s="5">
-        <v>437176.76</v>
+      <c r="W24" s="52">
+        <v>592637.84491726558</v>
       </c>
       <c r="X24" s="5">
         <v>597047.375</v>
@@ -39326,8 +39334,8 @@
       <c r="V25" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="W25" s="9">
-        <v>351653.1875</v>
+      <c r="W25" s="51">
+        <v>348127.70535714302</v>
       </c>
       <c r="X25" s="9">
         <v>351653.1875</v>
@@ -39431,8 +39439,8 @@
       <c r="V26" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="W26" s="9">
-        <v>0</v>
+      <c r="W26" s="51">
+        <v>158986.56926012269</v>
       </c>
       <c r="X26" s="9">
         <v>159870.5938</v>
@@ -42964,8 +42972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView topLeftCell="G25" workbookViewId="0">
-      <selection activeCell="Q55" sqref="A3:X63"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Implemented metrics until SPI(t),
TODO: p-factor and EVM forecastings
</commit_message>
<xml_diff>
--- a/PMConverter/administration/2_Project data input sheet_extended_checked.xlsx
+++ b/PMConverter/administration/2_Project data input sheet_extended_checked.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36165" yWindow="-5595" windowWidth="29340" windowHeight="16440" tabRatio="628" activeTab="8"/>
+    <workbookView xWindow="-36165" yWindow="-5595" windowWidth="29340" windowHeight="16440" tabRatio="628" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline Schedule" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="TP6" sheetId="9" r:id="rId9"/>
     <sheet name="TP7" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1745,6 +1745,12 @@
     <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1756,12 +1762,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="120">
@@ -2306,30 +2306,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47" t="s">
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47" t="s">
+      <c r="J1" s="49"/>
+      <c r="K1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
     </row>
     <row r="2" spans="1:17" ht="21">
       <c r="A2" s="2" t="s">
@@ -4830,15 +4830,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
     <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
@@ -4865,7 +4866,7 @@
         <v>391</v>
       </c>
       <c r="C1" s="33">
-        <v>39456.708333333336</v>
+        <v>39457.333333333336</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="13" t="s">
@@ -4876,40 +4877,40 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="AE3" t="s">
         <v>395</v>
       </c>
@@ -10703,20 +10704,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47" t="s">
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="47"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" ht="21">
       <c r="A2" s="2" t="s">
@@ -11088,19 +11089,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21">
-      <c r="A1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="47"/>
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49"/>
       <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="50" t="s">
         <v>389</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:7" ht="21">
       <c r="A2" s="2" t="s">
@@ -12422,7 +12423,7 @@
   <dimension ref="A1:BM63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="A3:X63"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12462,7 +12463,7 @@
         <v>391</v>
       </c>
       <c r="C1" s="20">
-        <v>38905.708333333336</v>
+        <v>38905.333333333336</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>392</v>
@@ -12472,48 +12473,48 @@
       </c>
     </row>
     <row r="3" spans="1:65">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="AI3" t="s">
         <v>395</v>
       </c>
-      <c r="BE3" s="47" t="s">
+      <c r="BE3" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="BF3" s="47"/>
-      <c r="BG3" s="47"/>
+      <c r="BF3" s="49"/>
+      <c r="BG3" s="49"/>
     </row>
     <row r="4" spans="1:65" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -20201,15 +20202,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
     <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
@@ -20235,7 +20237,7 @@
         <v>391</v>
       </c>
       <c r="C1" s="20">
-        <v>39121.708333333336</v>
+        <v>39121.333333333336</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>392</v>
@@ -20245,40 +20247,40 @@
       </c>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="AD3" t="s">
         <v>395</v>
       </c>
@@ -25808,15 +25810,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
     <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
@@ -25843,7 +25846,7 @@
         <v>391</v>
       </c>
       <c r="C1" s="20">
-        <v>39157.708333333336</v>
+        <v>39158.333333333336</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>392</v>
@@ -25853,40 +25856,40 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="AE3" t="s">
         <v>395</v>
       </c>
@@ -31512,8 +31515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK63"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -31547,7 +31550,7 @@
         <v>391</v>
       </c>
       <c r="C1" s="20">
-        <v>39234.708333333336</v>
+        <v>39237.333333333336</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>392</v>
@@ -31557,40 +31560,40 @@
       </c>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="AF3" t="s">
         <v>395</v>
       </c>
@@ -33046,7 +33049,7 @@
         <v>0.97</v>
       </c>
       <c r="V19" s="3"/>
-      <c r="W19" s="52">
+      <c r="W19" s="48">
         <v>528148.41970322584</v>
       </c>
       <c r="X19" s="5">
@@ -33133,7 +33136,7 @@
       <c r="V20" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="W20" s="51">
+      <c r="W20" s="47">
         <v>129606.87270322582</v>
       </c>
       <c r="X20" s="9">
@@ -37236,15 +37239,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
     <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
@@ -37272,7 +37276,7 @@
         <v>391</v>
       </c>
       <c r="C1" s="33">
-        <v>39262.708333333336</v>
+        <v>39265.333333333336</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="13" t="s">
@@ -37283,40 +37287,40 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="AE3" t="s">
         <v>395</v>
       </c>
@@ -39246,7 +39250,7 @@
         <v>0.99</v>
       </c>
       <c r="V24" s="3"/>
-      <c r="W24" s="52">
+      <c r="W24" s="48">
         <v>592637.84491726558</v>
       </c>
       <c r="X24" s="5">
@@ -39334,7 +39338,7 @@
       <c r="V25" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="W25" s="51">
+      <c r="W25" s="47">
         <v>348127.70535714302</v>
       </c>
       <c r="X25" s="9">
@@ -39439,7 +39443,7 @@
       <c r="V26" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="W26" s="51">
+      <c r="W26" s="47">
         <v>158986.56926012269</v>
       </c>
       <c r="X26" s="9">
@@ -42972,15 +42976,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Y33" sqref="Y33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
     <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
@@ -43005,7 +43010,7 @@
         <v>391</v>
       </c>
       <c r="C1" s="33">
-        <v>39379.708333333336</v>
+        <v>39379.333333333336</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="13" t="s">
@@ -43016,40 +43021,40 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="AE3" t="s">
         <v>395</v>
       </c>

</xml_diff>

<commit_message>
fixed general deriving of variables from p2x data
</commit_message>
<xml_diff>
--- a/PMConverter/administration/2_Project data input sheet_extended_checked.xlsx
+++ b/PMConverter/administration/2_Project data input sheet_extended_checked.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36165" yWindow="-5595" windowWidth="29340" windowHeight="16440" tabRatio="628" activeTab="9"/>
+    <workbookView xWindow="-36165" yWindow="-5595" windowWidth="29340" windowHeight="16440" tabRatio="628" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline Schedule" sheetId="1" r:id="rId1"/>
@@ -2286,7 +2286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
@@ -4830,7 +4830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -10688,7 +10688,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -11077,7 +11077,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12422,8 +12422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BM63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -25811,7 +25811,7 @@
   <dimension ref="A1:AJ63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -31516,7 +31516,7 @@
   <dimension ref="A1:AK63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -37240,7 +37240,7 @@
   <dimension ref="A1:AJ63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -42976,7 +42976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>